<commit_message>
output code samengevoegd. verdeelde belasting aangepast
</commit_message>
<xml_diff>
--- a/Main/Voorbeeldschip_Deelopdracht_8_V5.xlsx
+++ b/Main/Voorbeeldschip_Deelopdracht_8_V5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Surfdrive\MT1463enMT1466\Deelopdrachten\Deelopdracht 8\Voorbeeldschip_Deelopdracht_8\VoorbeeldschipV5 (01-04-2025)\Voorbeeldschip (01-04-2025)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/cmazel_tudelft_nl/Documents/Q3/integratie en vaardigheden/Deelopdracht8IenV/Main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966AE447-6F68-48EF-B09A-73DB34CB40F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{966AE447-6F68-48EF-B09A-73DB34CB40F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94DFD748-4EC2-4287-82DF-A1EC84466BA0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="13776" xr2:uid="{EDFD90E1-A827-4CFB-9BA4-06037854822A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{EDFD90E1-A827-4CFB-9BA4-06037854822A}"/>
   </bookViews>
   <sheets>
     <sheet name="AntwoordenbladV3 DO2schip" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
   </externalReferences>
   <definedNames>
     <definedName name="Aantal_WBTNK" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'AntwoordenbladV3 DO2schip'!$A$1:$D$142</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'AntwoordenbladV3 DO2schip'!$1:$1</definedName>
     <definedName name="Afwijking_F" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$49</definedName>
     <definedName name="Afwijking_M" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$50</definedName>
     <definedName name="Buoyancy" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$43</definedName>
@@ -40,8 +42,6 @@
     <definedName name="m_tp" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$67</definedName>
     <definedName name="Notes" localSheetId="0">'AntwoordenbladV3 DO2schip'!$B$100</definedName>
     <definedName name="NumberTP" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$66</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'AntwoordenbladV3 DO2schip'!$A$1:$D$142</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'AntwoordenbladV3 DO2schip'!$1:$1</definedName>
     <definedName name="Rhino" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$6</definedName>
     <definedName name="rho_staal" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$31</definedName>
     <definedName name="rho_water" localSheetId="0">'AntwoordenbladV3 DO2schip'!$B$32</definedName>
@@ -871,8 +871,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -901,28 +917,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="3" builtinId="10"/>
+    <cellStyle name="Controlecel" xfId="2" builtinId="23"/>
+    <cellStyle name="Invoer" xfId="1" builtinId="20"/>
+    <cellStyle name="Notitie" xfId="3" builtinId="10"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -1156,7 +1156,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1475,8 +1475,8 @@
   <dimension ref="A1:G142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,12 +1552,12 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -1588,24 +1588,24 @@
       <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="27">
         <v>470.55</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="35.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
     </row>
     <row r="15" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
@@ -1630,20 +1630,20 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
     </row>
     <row r="18" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="7"/>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -1657,19 +1657,19 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
@@ -1793,19 +1793,19 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
     </row>
     <row r="34" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="s">
@@ -1863,11 +1863,11 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
@@ -1925,11 +1925,11 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
@@ -1965,19 +1965,19 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
     </row>
     <row r="53" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="38" t="s">
+      <c r="B53" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
     </row>
     <row r="54" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="9" t="s">
@@ -2046,33 +2046,33 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="39" t="s">
+      <c r="B60" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="39"/>
-      <c r="D60" s="40"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="33"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="41"/>
-      <c r="D61" s="41"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
     </row>
     <row r="62" spans="1:4" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
     </row>
     <row r="63" spans="1:4" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="27" t="s">
+      <c r="B63" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B64" s="9" t="s">
@@ -2331,20 +2331,20 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="37" t="s">
+      <c r="A90" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="37"/>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
+      <c r="B90" s="28"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
     </row>
     <row r="91" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="7"/>
-      <c r="B91" s="27" t="s">
+      <c r="B91" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29"/>
     </row>
     <row r="92" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="17" t="s">
@@ -2426,59 +2426,59 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B100" s="28" t="s">
+      <c r="B100" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="C100" s="29"/>
-      <c r="D100" s="30"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="36"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B101" s="31"/>
-      <c r="C101" s="32"/>
-      <c r="D101" s="33"/>
+      <c r="B101" s="37"/>
+      <c r="C101" s="38"/>
+      <c r="D101" s="39"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B102" s="31"/>
-      <c r="C102" s="32"/>
-      <c r="D102" s="33"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="39"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B103" s="31"/>
-      <c r="C103" s="32"/>
-      <c r="D103" s="33"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="39"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B104" s="31"/>
-      <c r="C104" s="32"/>
-      <c r="D104" s="33"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="39"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B105" s="31"/>
-      <c r="C105" s="32"/>
-      <c r="D105" s="33"/>
+      <c r="B105" s="37"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="39"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B106" s="31"/>
-      <c r="C106" s="32"/>
-      <c r="D106" s="33"/>
+      <c r="B106" s="37"/>
+      <c r="C106" s="38"/>
+      <c r="D106" s="39"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B107" s="31"/>
-      <c r="C107" s="32"/>
-      <c r="D107" s="33"/>
+      <c r="B107" s="37"/>
+      <c r="C107" s="38"/>
+      <c r="D107" s="39"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B108" s="34"/>
-      <c r="C108" s="35"/>
-      <c r="D108" s="36"/>
+      <c r="B108" s="40"/>
+      <c r="C108" s="41"/>
+      <c r="D108" s="42"/>
     </row>
     <row r="109" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A109" s="37" t="s">
+      <c r="A109" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B109" s="37"/>
-      <c r="C109" s="37"/>
-      <c r="D109" s="37"/>
+      <c r="B109" s="28"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="28"/>
     </row>
     <row r="110" spans="1:7" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A110" s="7"/>
@@ -2714,27 +2714,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B100:D108"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B48:D48"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B100:D108"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="B91:D91"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Saus en nog meer saus
</commit_message>
<xml_diff>
--- a/Main/Voorbeeldschip_Deelopdracht_8_V5.xlsx
+++ b/Main/Voorbeeldschip_Deelopdracht_8_V5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/cmazel_tudelft_nl/Documents/Q3/integratie en vaardigheden/Deelopdracht8IenV/Main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Surfdrive\MT1463enMT1466\Deelopdrachten\Deelopdracht 8\Voorbeeldschip_Deelopdracht_8\VoorbeeldschipV5 (01-04-2025)\Voorbeeldschip (01-04-2025)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{966AE447-6F68-48EF-B09A-73DB34CB40F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94DFD748-4EC2-4287-82DF-A1EC84466BA0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966AE447-6F68-48EF-B09A-73DB34CB40F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{EDFD90E1-A827-4CFB-9BA4-06037854822A}"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="13776" xr2:uid="{EDFD90E1-A827-4CFB-9BA4-06037854822A}"/>
   </bookViews>
   <sheets>
     <sheet name="AntwoordenbladV3 DO2schip" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,6 @@
   </externalReferences>
   <definedNames>
     <definedName name="Aantal_WBTNK" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$28</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'AntwoordenbladV3 DO2schip'!$A$1:$D$142</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'AntwoordenbladV3 DO2schip'!$1:$1</definedName>
     <definedName name="Afwijking_F" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$49</definedName>
     <definedName name="Afwijking_M" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$50</definedName>
     <definedName name="Buoyancy" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$43</definedName>
@@ -42,6 +40,8 @@
     <definedName name="m_tp" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$67</definedName>
     <definedName name="Notes" localSheetId="0">'AntwoordenbladV3 DO2schip'!$B$100</definedName>
     <definedName name="NumberTP" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$66</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'AntwoordenbladV3 DO2schip'!$A$1:$D$142</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'AntwoordenbladV3 DO2schip'!$1:$1</definedName>
     <definedName name="Rhino" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$6</definedName>
     <definedName name="rho_staal" localSheetId="0">'AntwoordenbladV3 DO2schip'!$D$31</definedName>
     <definedName name="rho_water" localSheetId="0">'AntwoordenbladV3 DO2schip'!$B$32</definedName>
@@ -871,24 +871,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -917,12 +901,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Controlecel" xfId="2" builtinId="23"/>
-    <cellStyle name="Invoer" xfId="1" builtinId="20"/>
-    <cellStyle name="Notitie" xfId="3" builtinId="10"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -1156,7 +1156,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1475,8 +1475,8 @@
   <dimension ref="A1:G142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,12 +1552,12 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -1588,24 +1588,24 @@
       <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="42">
         <v>470.55</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="35.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
@@ -1630,20 +1630,20 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="7"/>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -1657,19 +1657,19 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
@@ -1793,19 +1793,19 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
     </row>
     <row r="34" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="s">
@@ -1863,11 +1863,11 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
@@ -1925,11 +1925,11 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
@@ -1965,19 +1965,19 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
     </row>
     <row r="53" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
     </row>
     <row r="54" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="9" t="s">
@@ -2046,33 +2046,33 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="32"/>
-      <c r="D60" s="33"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="40"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
     </row>
     <row r="62" spans="1:4" ht="39.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
     </row>
     <row r="63" spans="1:4" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="29" t="s">
+      <c r="B63" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B64" s="9" t="s">
@@ -2331,20 +2331,20 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="28" t="s">
+      <c r="A90" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
     </row>
     <row r="91" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="7"/>
-      <c r="B91" s="29" t="s">
+      <c r="B91" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C91" s="29"/>
-      <c r="D91" s="29"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
     </row>
     <row r="92" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="17" t="s">
@@ -2426,59 +2426,59 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B100" s="34" t="s">
+      <c r="B100" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C100" s="35"/>
-      <c r="D100" s="36"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="30"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B101" s="37"/>
-      <c r="C101" s="38"/>
-      <c r="D101" s="39"/>
+      <c r="B101" s="31"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="33"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B102" s="37"/>
-      <c r="C102" s="38"/>
-      <c r="D102" s="39"/>
+      <c r="B102" s="31"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="33"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B103" s="37"/>
-      <c r="C103" s="38"/>
-      <c r="D103" s="39"/>
+      <c r="B103" s="31"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="33"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B104" s="37"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="39"/>
+      <c r="B104" s="31"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="33"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B105" s="37"/>
-      <c r="C105" s="38"/>
-      <c r="D105" s="39"/>
+      <c r="B105" s="31"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="33"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B106" s="37"/>
-      <c r="C106" s="38"/>
-      <c r="D106" s="39"/>
+      <c r="B106" s="31"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="33"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B107" s="37"/>
-      <c r="C107" s="38"/>
-      <c r="D107" s="39"/>
+      <c r="B107" s="31"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="33"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B108" s="40"/>
-      <c r="C108" s="41"/>
-      <c r="D108" s="42"/>
+      <c r="B108" s="34"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="36"/>
     </row>
     <row r="109" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A109" s="28" t="s">
+      <c r="A109" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="B109" s="28"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
+      <c r="B109" s="37"/>
+      <c r="C109" s="37"/>
+      <c r="D109" s="37"/>
     </row>
     <row r="110" spans="1:7" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A110" s="7"/>
@@ -2714,27 +2714,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B100:D108"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B48:D48"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B100:D108"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="B91:D91"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>

</xml_diff>